<commit_message>
better bundle example explanation
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.imaging.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.imaging.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-30T12:22:18-05:00</t>
+    <t>2023-03-31T07:50:38-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -87,8 +87,9 @@
     <t>A profile on the DocumentReference resource for MHV PHR exposing Radiology note (ImagingExamTO) using FHIR API.
 - The mock example maps best to VIA_v4.0.7_uat.wsdl. 
 - based on US-Core for Clinical Notes
-- type LOINC#18748-4 "Diagnostic imaging study"
+- type LOINC#18748-4 `Diagnostic imaging study`
 - see [mapping](StructureDefinition-VA.MHV.PHR.imaging-mappings.html#mappings-for-vdif-to-mhv-phr-imagingexamto) for details
+- An example of a [transaction Bundle](Bundle-images.html) with many image reports as DocumentReference. This was [transformed using the included XSLT](StructureDefinition-VA.MHV.PHR.imaging.html#notes) from the [mock sample SOAP message](https://github.com/JohnMoehrke/MHV-PHR/blob/main/mocks/radiology.xml) MHV receives.
 TODO Questions:
 - some schema elements found in VIA_v4.0.7_uat.wsdl are not mapped here because I can't tell what is in them. Most of them likely have a place to go in the FHIR model, but I need to know more about them.
   - hasImages

</xml_diff>